<commit_message>
Added aerosol and chemistry information and modified the atmosphere sheet
</commit_message>
<xml_diff>
--- a/cmip6/models/noresm2-lm/cmip6_ncc_noresm2-lm_aerosol.xlsx
+++ b/cmip6/models/noresm2-lm/cmip6_ncc_noresm2-lm_aerosol.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="530">
   <si>
     <t xml:space="preserve">ES-DOC CMIP6 Model Documentation</t>
   </si>
@@ -1144,6 +1144,47 @@
   </si>
   <si>
     <t xml:space="preserve">cmip6.aerosol.optical_radiative_properties.overview</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">See description in overview for how the radiative properties are calculated. BC, DUST and OM are all absorbing. The complex refractive indices given below
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+SS : 1.5 + 1.0E-8 i 
+DUST: 1.53 + 2.4E-3 i
+SO4: 1.43 + 1.0E-8 i
+OM: 1.53 + 6E-3 i
+BC: 1.59 + 0.79 i
+H2O: 1.333 + 1.96E-9 I
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">6.2.1</t>
@@ -1631,7 +1672,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1766,6 +1807,21 @@
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val=""/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val=""/>
+      <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -2244,7 +2300,7 @@
   </sheetPr>
   <dimension ref="A1:AI146"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B127" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B114" activeCellId="0" sqref="B114"/>
     </sheetView>
   </sheetViews>
@@ -3216,7 +3272,7 @@
   </sheetPr>
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
     </sheetView>
   </sheetViews>
@@ -3719,7 +3775,7 @@
   </sheetPr>
   <dimension ref="A1:AI52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
     </sheetView>
   </sheetViews>
@@ -4178,7 +4234,7 @@
   </sheetPr>
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -4250,7 +4306,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="178" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="11" t="s">
         <v>341</v>
       </c>
     </row>
@@ -4384,8 +4440,8 @@
   </sheetPr>
   <dimension ref="A1:C105"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4429,7 +4485,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="11" t="s">
         <v>366</v>
       </c>
     </row>
@@ -4458,38 +4514,42 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="178" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="11"/>
-    </row>
+      <c r="B11" s="16" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="12" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="13" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="14" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4497,21 +4557,21 @@
     </row>
     <row r="21" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="14" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4519,21 +4579,21 @@
     </row>
     <row r="25" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="14" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4541,10 +4601,10 @@
     </row>
     <row r="30" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="12" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4552,10 +4612,10 @@
     </row>
     <row r="33" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="9" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4563,10 +4623,10 @@
         <v>89</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4577,10 +4637,10 @@
     </row>
     <row r="37" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4588,10 +4648,10 @@
         <v>89</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4602,10 +4662,10 @@
     </row>
     <row r="41" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="9" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4613,36 +4673,36 @@
         <v>43</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B43" s="16" t="s">
-        <v>400</v>
+      <c r="B43" s="11" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="12" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B47" s="13" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4650,10 +4710,10 @@
         <v>89</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4664,10 +4724,10 @@
     </row>
     <row r="53" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="9" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4675,23 +4735,24 @@
         <v>89</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B55" s="15" t="b">
+      <c r="B55" s="15" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="9" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4699,33 +4760,34 @@
         <v>89</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B59" s="15" t="b">
+      <c r="B59" s="15" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="12" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B63" s="13" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="9" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B65" s="9" t="s">
         <v>54</v>
@@ -4736,10 +4798,10 @@
         <v>43</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4748,16 +4810,16 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="178" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B68" s="16" t="s">
-        <v>422</v>
+      <c r="B68" s="11" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="9" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4765,10 +4827,10 @@
         <v>84</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4778,10 +4840,10 @@
     </row>
     <row r="74" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="9" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4789,10 +4851,10 @@
         <v>84</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4802,20 +4864,20 @@
     </row>
     <row r="79" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="12" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B80" s="13" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="9" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B82" s="9" t="s">
         <v>54</v>
@@ -4826,10 +4888,10 @@
         <v>43</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C83" s="10" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4842,10 +4904,10 @@
     </row>
     <row r="87" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="9" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4853,10 +4915,10 @@
         <v>89</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C88" s="10" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4867,10 +4929,10 @@
     </row>
     <row r="91" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="9" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4878,10 +4940,10 @@
         <v>84</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C92" s="10" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4891,10 +4953,10 @@
     </row>
     <row r="95" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="9" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4902,10 +4964,10 @@
         <v>89</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C96" s="10" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4916,10 +4978,10 @@
     </row>
     <row r="99" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="9" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4927,21 +4989,23 @@
         <v>89</v>
       </c>
       <c r="B100" s="10" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C100" s="10" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B101" s="11"/>
+      <c r="B101" s="15" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="103" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="9" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4949,14 +5013,16 @@
         <v>84</v>
       </c>
       <c r="B104" s="10" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C104" s="10" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B105" s="11"/>
+      <c r="B105" s="11" t="n">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="15">
@@ -5038,7 +5104,7 @@
   </sheetPr>
   <dimension ref="A1:AN54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -5052,7 +5118,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>5</v>
@@ -5060,12 +5126,12 @@
     </row>
     <row r="2" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="13" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>42</v>
@@ -5076,20 +5142,20 @@
         <v>43</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="11" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>54</v>
@@ -5100,10 +5166,10 @@
         <v>43</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5113,15 +5179,15 @@
     </row>
     <row r="11" customFormat="false" ht="178" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="11" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5129,10 +5195,10 @@
         <v>61</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5142,582 +5208,582 @@
     </row>
     <row r="16" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="11" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="AA16" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="AB16" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="AC16" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="AD16" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="AE16" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="AF16" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="AG16" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="AH16" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="AI16" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="AJ16" s="6" t="s">
         <v>470</v>
       </c>
-      <c r="AB16" s="6" t="s">
-        <v>471</v>
-      </c>
-      <c r="AC16" s="6" t="s">
-        <v>472</v>
-      </c>
-      <c r="AD16" s="6" t="s">
-        <v>473</v>
-      </c>
-      <c r="AE16" s="6" t="s">
-        <v>474</v>
-      </c>
-      <c r="AF16" s="6" t="s">
-        <v>475</v>
-      </c>
-      <c r="AG16" s="6" t="s">
-        <v>476</v>
-      </c>
-      <c r="AH16" s="6" t="s">
-        <v>477</v>
-      </c>
-      <c r="AI16" s="6" t="s">
-        <v>478</v>
-      </c>
-      <c r="AJ16" s="6" t="s">
-        <v>469</v>
-      </c>
       <c r="AK16" s="6" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="AL16" s="6" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="AM16" s="6" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B17" s="11" t="s">
+        <v>480</v>
+      </c>
+      <c r="AA17" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="AB17" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="AC17" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="AD17" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="AE17" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="AF17" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="AG17" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="AH17" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="AI17" s="6" t="s">
         <v>479</v>
       </c>
-      <c r="AA17" s="6" t="s">
+      <c r="AJ17" s="6" t="s">
         <v>470</v>
       </c>
-      <c r="AB17" s="6" t="s">
-        <v>471</v>
-      </c>
-      <c r="AC17" s="6" t="s">
-        <v>472</v>
-      </c>
-      <c r="AD17" s="6" t="s">
-        <v>473</v>
-      </c>
-      <c r="AE17" s="6" t="s">
-        <v>474</v>
-      </c>
-      <c r="AF17" s="6" t="s">
-        <v>475</v>
-      </c>
-      <c r="AG17" s="6" t="s">
-        <v>476</v>
-      </c>
-      <c r="AH17" s="6" t="s">
-        <v>477</v>
-      </c>
-      <c r="AI17" s="6" t="s">
-        <v>478</v>
-      </c>
-      <c r="AJ17" s="6" t="s">
-        <v>469</v>
-      </c>
       <c r="AK17" s="6" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="AL17" s="6" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="AM17" s="6" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="11" t="s">
+        <v>475</v>
+      </c>
+      <c r="AA18" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="AB18" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="AC18" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="AD18" s="6" t="s">
         <v>474</v>
       </c>
-      <c r="AA18" s="6" t="s">
+      <c r="AE18" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="AF18" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="AG18" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="AH18" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="AI18" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="AJ18" s="6" t="s">
         <v>470</v>
       </c>
-      <c r="AB18" s="6" t="s">
-        <v>471</v>
-      </c>
-      <c r="AC18" s="6" t="s">
-        <v>472</v>
-      </c>
-      <c r="AD18" s="6" t="s">
-        <v>473</v>
-      </c>
-      <c r="AE18" s="6" t="s">
-        <v>474</v>
-      </c>
-      <c r="AF18" s="6" t="s">
-        <v>475</v>
-      </c>
-      <c r="AG18" s="6" t="s">
-        <v>476</v>
-      </c>
-      <c r="AH18" s="6" t="s">
-        <v>477</v>
-      </c>
-      <c r="AI18" s="6" t="s">
-        <v>478</v>
-      </c>
-      <c r="AJ18" s="6" t="s">
-        <v>469</v>
-      </c>
       <c r="AK18" s="6" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="AL18" s="6" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="AM18" s="6" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="11" t="s">
+        <v>478</v>
+      </c>
+      <c r="AA19" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="AB19" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="AC19" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="AD19" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="AE19" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="AF19" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="AG19" s="6" t="s">
         <v>477</v>
       </c>
-      <c r="AA19" s="6" t="s">
+      <c r="AH19" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="AI19" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="AJ19" s="6" t="s">
         <v>470</v>
       </c>
-      <c r="AB19" s="6" t="s">
-        <v>471</v>
-      </c>
-      <c r="AC19" s="6" t="s">
-        <v>472</v>
-      </c>
-      <c r="AD19" s="6" t="s">
-        <v>473</v>
-      </c>
-      <c r="AE19" s="6" t="s">
-        <v>474</v>
-      </c>
-      <c r="AF19" s="6" t="s">
-        <v>475</v>
-      </c>
-      <c r="AG19" s="6" t="s">
-        <v>476</v>
-      </c>
-      <c r="AH19" s="6" t="s">
-        <v>477</v>
-      </c>
-      <c r="AI19" s="6" t="s">
-        <v>478</v>
-      </c>
-      <c r="AJ19" s="6" t="s">
-        <v>469</v>
-      </c>
       <c r="AK19" s="6" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="AL19" s="6" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="AM19" s="6" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="11" t="s">
+        <v>471</v>
+      </c>
+      <c r="AA20" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="AB20" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="AC20" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="AD20" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="AE20" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="AF20" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="AG20" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="AH20" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="AI20" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="AJ20" s="6" t="s">
         <v>470</v>
       </c>
-      <c r="AA20" s="6" t="s">
-        <v>470</v>
-      </c>
-      <c r="AB20" s="6" t="s">
-        <v>471</v>
-      </c>
-      <c r="AC20" s="6" t="s">
-        <v>472</v>
-      </c>
-      <c r="AD20" s="6" t="s">
-        <v>473</v>
-      </c>
-      <c r="AE20" s="6" t="s">
-        <v>474</v>
-      </c>
-      <c r="AF20" s="6" t="s">
-        <v>475</v>
-      </c>
-      <c r="AG20" s="6" t="s">
-        <v>476</v>
-      </c>
-      <c r="AH20" s="6" t="s">
-        <v>477</v>
-      </c>
-      <c r="AI20" s="6" t="s">
-        <v>478</v>
-      </c>
-      <c r="AJ20" s="6" t="s">
-        <v>469</v>
-      </c>
       <c r="AK20" s="6" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="AL20" s="6" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="AM20" s="6" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="11" t="s">
+        <v>476</v>
+      </c>
+      <c r="AA21" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="AB21" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="AC21" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="AD21" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="AE21" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="AA21" s="6" t="s">
+      <c r="AF21" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="AG21" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="AH21" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="AI21" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="AJ21" s="6" t="s">
         <v>470</v>
       </c>
-      <c r="AB21" s="6" t="s">
-        <v>471</v>
-      </c>
-      <c r="AC21" s="6" t="s">
-        <v>472</v>
-      </c>
-      <c r="AD21" s="6" t="s">
-        <v>473</v>
-      </c>
-      <c r="AE21" s="6" t="s">
-        <v>474</v>
-      </c>
-      <c r="AF21" s="6" t="s">
-        <v>475</v>
-      </c>
-      <c r="AG21" s="6" t="s">
-        <v>476</v>
-      </c>
-      <c r="AH21" s="6" t="s">
-        <v>477</v>
-      </c>
-      <c r="AI21" s="6" t="s">
-        <v>478</v>
-      </c>
-      <c r="AJ21" s="6" t="s">
-        <v>469</v>
-      </c>
       <c r="AK21" s="6" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="AL21" s="6" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="AM21" s="6" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="11" t="s">
+        <v>477</v>
+      </c>
+      <c r="AA22" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="AB22" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="AC22" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="AD22" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="AE22" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="AF22" s="6" t="s">
         <v>476</v>
       </c>
-      <c r="AA22" s="6" t="s">
+      <c r="AG22" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="AH22" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="AI22" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="AJ22" s="6" t="s">
         <v>470</v>
       </c>
-      <c r="AB22" s="6" t="s">
-        <v>471</v>
-      </c>
-      <c r="AC22" s="6" t="s">
-        <v>472</v>
-      </c>
-      <c r="AD22" s="6" t="s">
-        <v>473</v>
-      </c>
-      <c r="AE22" s="6" t="s">
-        <v>474</v>
-      </c>
-      <c r="AF22" s="6" t="s">
-        <v>475</v>
-      </c>
-      <c r="AG22" s="6" t="s">
-        <v>476</v>
-      </c>
-      <c r="AH22" s="6" t="s">
-        <v>477</v>
-      </c>
-      <c r="AI22" s="6" t="s">
-        <v>478</v>
-      </c>
-      <c r="AJ22" s="6" t="s">
-        <v>469</v>
-      </c>
       <c r="AK22" s="6" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="AL22" s="6" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="AM22" s="6" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="11" t="s">
+        <v>472</v>
+      </c>
+      <c r="AA23" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="AA23" s="6" t="s">
+      <c r="AB23" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="AC23" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="AD23" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="AE23" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="AF23" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="AG23" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="AH23" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="AI23" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="AJ23" s="6" t="s">
         <v>470</v>
       </c>
-      <c r="AB23" s="6" t="s">
-        <v>471</v>
-      </c>
-      <c r="AC23" s="6" t="s">
-        <v>472</v>
-      </c>
-      <c r="AD23" s="6" t="s">
-        <v>473</v>
-      </c>
-      <c r="AE23" s="6" t="s">
-        <v>474</v>
-      </c>
-      <c r="AF23" s="6" t="s">
-        <v>475</v>
-      </c>
-      <c r="AG23" s="6" t="s">
-        <v>476</v>
-      </c>
-      <c r="AH23" s="6" t="s">
-        <v>477</v>
-      </c>
-      <c r="AI23" s="6" t="s">
-        <v>478</v>
-      </c>
-      <c r="AJ23" s="6" t="s">
-        <v>469</v>
-      </c>
       <c r="AK23" s="6" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="AL23" s="6" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="AM23" s="6" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="11" t="s">
+        <v>473</v>
+      </c>
+      <c r="AA24" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="AB24" s="6" t="s">
         <v>472</v>
       </c>
-      <c r="AA24" s="6" t="s">
+      <c r="AC24" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="AD24" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="AE24" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="AF24" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="AG24" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="AH24" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="AI24" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="AJ24" s="6" t="s">
         <v>470</v>
       </c>
-      <c r="AB24" s="6" t="s">
-        <v>471</v>
-      </c>
-      <c r="AC24" s="6" t="s">
-        <v>472</v>
-      </c>
-      <c r="AD24" s="6" t="s">
-        <v>473</v>
-      </c>
-      <c r="AE24" s="6" t="s">
-        <v>474</v>
-      </c>
-      <c r="AF24" s="6" t="s">
-        <v>475</v>
-      </c>
-      <c r="AG24" s="6" t="s">
-        <v>476</v>
-      </c>
-      <c r="AH24" s="6" t="s">
-        <v>477</v>
-      </c>
-      <c r="AI24" s="6" t="s">
-        <v>478</v>
-      </c>
-      <c r="AJ24" s="6" t="s">
-        <v>469</v>
-      </c>
       <c r="AK24" s="6" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="AL24" s="6" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="AM24" s="6" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="11" t="s">
+        <v>474</v>
+      </c>
+      <c r="AA25" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="AB25" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="AC25" s="6" t="s">
         <v>473</v>
       </c>
-      <c r="AA25" s="6" t="s">
+      <c r="AD25" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="AE25" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="AF25" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="AG25" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="AH25" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="AI25" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="AJ25" s="6" t="s">
         <v>470</v>
       </c>
-      <c r="AB25" s="6" t="s">
-        <v>471</v>
-      </c>
-      <c r="AC25" s="6" t="s">
-        <v>472</v>
-      </c>
-      <c r="AD25" s="6" t="s">
-        <v>473</v>
-      </c>
-      <c r="AE25" s="6" t="s">
-        <v>474</v>
-      </c>
-      <c r="AF25" s="6" t="s">
-        <v>475</v>
-      </c>
-      <c r="AG25" s="6" t="s">
-        <v>476</v>
-      </c>
-      <c r="AH25" s="6" t="s">
-        <v>477</v>
-      </c>
-      <c r="AI25" s="6" t="s">
-        <v>478</v>
-      </c>
-      <c r="AJ25" s="6" t="s">
-        <v>469</v>
-      </c>
       <c r="AK25" s="6" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="AL25" s="6" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="AM25" s="6" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="11" t="s">
+        <v>482</v>
+      </c>
+      <c r="AA26" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="AB26" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="AC26" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="AD26" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="AE26" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="AF26" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="AG26" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="AH26" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="AI26" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="AJ26" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="AK26" s="6" t="s">
+        <v>480</v>
+      </c>
+      <c r="AL26" s="6" t="s">
         <v>481</v>
       </c>
-      <c r="AA26" s="6" t="s">
-        <v>470</v>
-      </c>
-      <c r="AB26" s="6" t="s">
-        <v>471</v>
-      </c>
-      <c r="AC26" s="6" t="s">
-        <v>472</v>
-      </c>
-      <c r="AD26" s="6" t="s">
-        <v>473</v>
-      </c>
-      <c r="AE26" s="6" t="s">
-        <v>474</v>
-      </c>
-      <c r="AF26" s="6" t="s">
-        <v>475</v>
-      </c>
-      <c r="AG26" s="6" t="s">
-        <v>476</v>
-      </c>
-      <c r="AH26" s="6" t="s">
-        <v>477</v>
-      </c>
-      <c r="AI26" s="6" t="s">
-        <v>478</v>
-      </c>
-      <c r="AJ26" s="6" t="s">
-        <v>469</v>
-      </c>
-      <c r="AK26" s="6" t="s">
-        <v>479</v>
-      </c>
-      <c r="AL26" s="6" t="s">
-        <v>480</v>
-      </c>
       <c r="AM26" s="6" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="11" t="s">
+        <v>481</v>
+      </c>
+      <c r="AA27" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="AB27" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="AC27" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="AD27" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="AE27" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="AF27" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="AG27" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="AH27" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="AI27" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="AJ27" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="AK27" s="6" t="s">
         <v>480</v>
       </c>
-      <c r="AA27" s="6" t="s">
-        <v>470</v>
-      </c>
-      <c r="AB27" s="6" t="s">
-        <v>471</v>
-      </c>
-      <c r="AC27" s="6" t="s">
-        <v>472</v>
-      </c>
-      <c r="AD27" s="6" t="s">
-        <v>473</v>
-      </c>
-      <c r="AE27" s="6" t="s">
-        <v>474</v>
-      </c>
-      <c r="AF27" s="6" t="s">
-        <v>475</v>
-      </c>
-      <c r="AG27" s="6" t="s">
-        <v>476</v>
-      </c>
-      <c r="AH27" s="6" t="s">
-        <v>477</v>
-      </c>
-      <c r="AI27" s="6" t="s">
-        <v>478</v>
-      </c>
-      <c r="AJ27" s="6" t="s">
-        <v>469</v>
-      </c>
-      <c r="AK27" s="6" t="s">
-        <v>479</v>
-      </c>
       <c r="AL27" s="6" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="AM27" s="6" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="11" t="s">
+        <v>479</v>
+      </c>
+      <c r="AA28" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="AB28" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="AC28" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="AD28" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="AE28" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="AF28" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="AG28" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="AH28" s="6" t="s">
         <v>478</v>
       </c>
-      <c r="AA28" s="6" t="s">
+      <c r="AI28" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="AJ28" s="6" t="s">
         <v>470</v>
       </c>
-      <c r="AB28" s="6" t="s">
-        <v>471</v>
-      </c>
-      <c r="AC28" s="6" t="s">
-        <v>472</v>
-      </c>
-      <c r="AD28" s="6" t="s">
-        <v>473</v>
-      </c>
-      <c r="AE28" s="6" t="s">
-        <v>474</v>
-      </c>
-      <c r="AF28" s="6" t="s">
-        <v>475</v>
-      </c>
-      <c r="AG28" s="6" t="s">
-        <v>476</v>
-      </c>
-      <c r="AH28" s="6" t="s">
-        <v>477</v>
-      </c>
-      <c r="AI28" s="6" t="s">
-        <v>478</v>
-      </c>
-      <c r="AJ28" s="6" t="s">
-        <v>469</v>
-      </c>
       <c r="AK28" s="6" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="AL28" s="6" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="AM28" s="6" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5725,10 +5791,10 @@
         <v>61</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5738,28 +5804,28 @@
     </row>
     <row r="33" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="11" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="AA33" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="AB33" s="6" t="s">
+        <v>489</v>
+      </c>
+      <c r="AC33" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="AD33" s="6" t="s">
         <v>487</v>
       </c>
-      <c r="AB33" s="6" t="s">
-        <v>488</v>
-      </c>
-      <c r="AC33" s="6" t="s">
-        <v>480</v>
-      </c>
-      <c r="AD33" s="6" t="s">
-        <v>486</v>
-      </c>
       <c r="AE33" s="6" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="AF33" s="6" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="AG33" s="6" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="AH33" s="6" t="s">
         <v>69</v>
@@ -5767,28 +5833,28 @@
     </row>
     <row r="34" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B34" s="11" t="s">
+        <v>493</v>
+      </c>
+      <c r="AA34" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="AB34" s="6" t="s">
+        <v>489</v>
+      </c>
+      <c r="AC34" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="AD34" s="6" t="s">
+        <v>487</v>
+      </c>
+      <c r="AE34" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="AF34" s="6" t="s">
+        <v>491</v>
+      </c>
+      <c r="AG34" s="6" t="s">
         <v>492</v>
-      </c>
-      <c r="AA34" s="6" t="s">
-        <v>487</v>
-      </c>
-      <c r="AB34" s="6" t="s">
-        <v>488</v>
-      </c>
-      <c r="AC34" s="6" t="s">
-        <v>480</v>
-      </c>
-      <c r="AD34" s="6" t="s">
-        <v>486</v>
-      </c>
-      <c r="AE34" s="6" t="s">
-        <v>489</v>
-      </c>
-      <c r="AF34" s="6" t="s">
-        <v>490</v>
-      </c>
-      <c r="AG34" s="6" t="s">
-        <v>491</v>
       </c>
       <c r="AH34" s="6" t="s">
         <v>69</v>
@@ -5796,28 +5862,28 @@
     </row>
     <row r="35" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B35" s="11" t="s">
+        <v>488</v>
+      </c>
+      <c r="AA35" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="AB35" s="6" t="s">
+        <v>489</v>
+      </c>
+      <c r="AC35" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="AD35" s="6" t="s">
         <v>487</v>
       </c>
-      <c r="AA35" s="6" t="s">
-        <v>487</v>
-      </c>
-      <c r="AB35" s="6" t="s">
-        <v>488</v>
-      </c>
-      <c r="AC35" s="6" t="s">
-        <v>480</v>
-      </c>
-      <c r="AD35" s="6" t="s">
-        <v>486</v>
-      </c>
       <c r="AE35" s="6" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="AF35" s="6" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="AG35" s="6" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="AH35" s="6" t="s">
         <v>69</v>
@@ -5825,10 +5891,10 @@
     </row>
     <row r="37" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5836,10 +5902,10 @@
         <v>61</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5849,31 +5915,31 @@
     </row>
     <row r="40" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B40" s="11" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="AA40" s="6" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="AB40" s="6" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="AC40" s="6" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="AD40" s="6" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="AE40" s="6" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="AF40" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="AG40" s="6" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="AH40" s="6" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="AI40" s="6" t="s">
         <v>69</v>
@@ -5881,31 +5947,31 @@
     </row>
     <row r="41" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B41" s="11" t="s">
+        <v>499</v>
+      </c>
+      <c r="AA41" s="6" t="s">
         <v>498</v>
       </c>
-      <c r="AA41" s="6" t="s">
-        <v>497</v>
-      </c>
       <c r="AB41" s="6" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="AC41" s="6" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="AD41" s="6" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="AE41" s="6" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="AF41" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="AG41" s="6" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="AH41" s="6" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="AI41" s="6" t="s">
         <v>69</v>
@@ -5913,31 +5979,31 @@
     </row>
     <row r="42" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B42" s="11" t="s">
+        <v>503</v>
+      </c>
+      <c r="AA42" s="6" t="s">
+        <v>498</v>
+      </c>
+      <c r="AB42" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="AC42" s="6" t="s">
+        <v>500</v>
+      </c>
+      <c r="AD42" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="AE42" s="6" t="s">
         <v>502</v>
       </c>
-      <c r="AA42" s="6" t="s">
-        <v>497</v>
-      </c>
-      <c r="AB42" s="6" t="s">
-        <v>498</v>
-      </c>
-      <c r="AC42" s="6" t="s">
-        <v>499</v>
-      </c>
-      <c r="AD42" s="6" t="s">
-        <v>500</v>
-      </c>
-      <c r="AE42" s="6" t="s">
-        <v>501</v>
-      </c>
       <c r="AF42" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="AG42" s="6" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="AH42" s="6" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="AI42" s="6" t="s">
         <v>69</v>
@@ -5945,31 +6011,31 @@
     </row>
     <row r="43" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B43" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="AA43" s="6" t="s">
+        <v>498</v>
+      </c>
+      <c r="AB43" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="AC43" s="6" t="s">
+        <v>500</v>
+      </c>
+      <c r="AD43" s="6" t="s">
         <v>501</v>
       </c>
-      <c r="AA43" s="6" t="s">
-        <v>497</v>
-      </c>
-      <c r="AB43" s="6" t="s">
-        <v>498</v>
-      </c>
-      <c r="AC43" s="6" t="s">
-        <v>499</v>
-      </c>
-      <c r="AD43" s="6" t="s">
-        <v>500</v>
-      </c>
       <c r="AE43" s="6" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="AF43" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="AG43" s="6" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="AH43" s="6" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="AI43" s="6" t="s">
         <v>69</v>
@@ -5977,31 +6043,31 @@
     </row>
     <row r="44" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B44" s="11" t="s">
+        <v>504</v>
+      </c>
+      <c r="AA44" s="6" t="s">
+        <v>498</v>
+      </c>
+      <c r="AB44" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="AC44" s="6" t="s">
+        <v>500</v>
+      </c>
+      <c r="AD44" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="AE44" s="6" t="s">
+        <v>502</v>
+      </c>
+      <c r="AF44" s="6" t="s">
         <v>503</v>
       </c>
-      <c r="AA44" s="6" t="s">
-        <v>497</v>
-      </c>
-      <c r="AB44" s="6" t="s">
-        <v>498</v>
-      </c>
-      <c r="AC44" s="6" t="s">
-        <v>499</v>
-      </c>
-      <c r="AD44" s="6" t="s">
-        <v>500</v>
-      </c>
-      <c r="AE44" s="6" t="s">
-        <v>501</v>
-      </c>
-      <c r="AF44" s="6" t="s">
-        <v>502</v>
-      </c>
       <c r="AG44" s="6" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="AH44" s="6" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="AI44" s="6" t="s">
         <v>69</v>
@@ -6009,10 +6075,10 @@
     </row>
     <row r="46" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="9" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6020,10 +6086,10 @@
         <v>61</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6036,16 +6102,16 @@
         <v>69</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="AA49" s="6" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="AB49" s="6" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="AC49" s="6" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="AD49" s="6" t="s">
         <v>69</v>
@@ -6053,10 +6119,10 @@
     </row>
     <row r="51" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="9" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6064,10 +6130,10 @@
         <v>61</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6078,43 +6144,43 @@
     <row r="54" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B54" s="11"/>
       <c r="AA54" s="6" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="AB54" s="6" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="AC54" s="6" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="AD54" s="6" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="AE54" s="6" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="AF54" s="6" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="AG54" s="6" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="AH54" s="6" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="AI54" s="6" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="AJ54" s="6" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="AK54" s="6" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="AL54" s="6" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="AM54" s="6" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="AN54" s="6" t="s">
         <v>69</v>

</xml_diff>